<commit_message>
Extend test for extract_dsp_from_excel + doc improvement.
</commit_message>
<xml_diff>
--- a/test/utils/example.xlsx
+++ b/test/utils/example.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27815"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/schedula/test/utils/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,8 +19,11 @@
   <definedNames>
     <definedName name="SINUS">Sheet1!$C$1:$C$18</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -62,6 +70,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -354,16 +367,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -380,7 +391,7 @@
         <v>-2.2863768173008364E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -392,8 +403,12 @@
         <f t="shared" si="1"/>
         <v>-0.99177885344311578</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2">
+        <f ca="1">SUM(INDIRECT("SINUS"))</f>
+        <v>-1.0914184244166338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -405,8 +420,12 @@
         <f t="shared" si="1"/>
         <v>0.92681850541778499</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" t="e">
+        <f ca="1">SQRT(D2)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -418,8 +437,12 @@
         <f t="shared" si="1"/>
         <v>0.9454451549211168</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4">
+        <f ca="1">INDIRECT("A1:A1")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -432,7 +455,7 @@
         <v>-0.68328372503552359</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
@@ -445,7 +468,7 @@
         <v>0.90176229056057366</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
@@ -458,7 +481,7 @@
         <v>0.86459689169594789</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
@@ -471,7 +494,7 @@
         <v>0.12372268789623808</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
@@ -484,7 +507,7 @@
         <v>-0.99975982007864272</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
@@ -497,7 +520,7 @@
         <v>0.97060061981194778</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11</v>
       </c>
@@ -510,7 +533,7 @@
         <v>0.98352241357378278</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>12</v>
       </c>
@@ -523,7 +546,7 @@
         <v>-0.91983693466953753</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>13</v>
       </c>
@@ -536,7 +559,7 @@
         <v>-0.90954815110388421</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>14</v>
       </c>
@@ -549,7 +572,7 @@
         <v>-0.9997715643824282</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>15</v>
       </c>
@@ -562,7 +585,7 @@
         <v>-0.71424378349544093</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
@@ -575,7 +598,7 @@
         <v>-0.44311307948133072</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>17</v>
       </c>
@@ -588,7 +611,7 @@
         <v>-0.80062916411734009</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>18</v>
       </c>
@@ -603,11 +626,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -617,14 +635,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <f ca="1">SUM(INDIRECT("Sheet1!A1:B18"))</f>
+        <v>680</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -634,13 +654,8 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FIX when a named range is not in the excel ref.
</commit_message>
<xml_diff>
--- a/test/utils/example.xlsx
+++ b/test/utils/example.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27815"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/schedula/test/utils/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="15600"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25515" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,11 +14,8 @@
   <definedNames>
     <definedName name="SINUS">Sheet1!$C$1:$C$18</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -367,11 +359,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -453,6 +447,10 @@
       <c r="C5">
         <f t="shared" si="1"/>
         <v>-0.68328372503552359</v>
+      </c>
+      <c r="D5" t="e">
+        <f ca="1">INDIRECT("invalid")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -635,7 +633,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1">
@@ -654,7 +652,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>